<commit_message>
Final Update I hope to god
</commit_message>
<xml_diff>
--- a/Management/Final Project Rubric.xlsx
+++ b/Management/Final Project Rubric.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive\Documents\GitHub\NBA-Database\Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adeel Asghar\Desktop\NBA-Database\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E188BA37-AC07-44E2-91E8-79D7692FADED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D058BCB-8AC6-4D97-AE44-03EB6F098B34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group rubrik" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Earned</t>
   </si>
@@ -121,16 +121,7 @@
     <t>Sequence type, location and purpose</t>
   </si>
   <si>
-    <t>Function name</t>
-  </si>
-  <si>
     <t>Location and purpose</t>
-  </si>
-  <si>
-    <t>Module name</t>
-  </si>
-  <si>
-    <t>Class name</t>
   </si>
   <si>
     <t>Machine description (screenshot)</t>
@@ -289,6 +280,27 @@
   </si>
   <si>
     <t>Excel spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bashaar Shah </t>
+  </si>
+  <si>
+    <t>gb2543</t>
+  </si>
+  <si>
+    <t>bashaarshah</t>
+  </si>
+  <si>
+    <t>00-50-56-C0-00-08</t>
+  </si>
+  <si>
+    <t>Function name : AddPlayer, DeletePlayer</t>
+  </si>
+  <si>
+    <t>30 excel sheets, each one for eacn NBA team</t>
+  </si>
+  <si>
+    <t>pandas</t>
   </si>
 </sst>
 </file>
@@ -433,7 +445,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -509,6 +521,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -622,6 +636,134 @@
         <a:xfrm>
           <a:off x="8751794" y="4226080"/>
           <a:ext cx="2151529" cy="3734519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>150869</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2141782</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>894714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF569D2D-5682-4360-8C4E-6A4AE1CA004F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11404173" y="3865217"/>
+          <a:ext cx="1990913" cy="894714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>135431</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>510164</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2336153</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2648558</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1287182D-E4A9-4538-8770-B7FC2CAB3BE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11388735" y="4375381"/>
+          <a:ext cx="2200722" cy="2138394"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2655969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2338306</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4350829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F62D19-9C53-4292-82D7-4B91F946EDBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11253304" y="6521186"/>
+          <a:ext cx="2338306" cy="1694860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -932,134 +1074,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C40D522-ECA1-FF4D-B661-39278A20B6C5}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="69" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2"/>
     <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="2"/>
+    <col min="6" max="6" width="48.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
       <c r="F1" s="31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1"/>
       <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1"/>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1219,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -1089,10 +1231,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1104,10 +1246,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1119,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -1134,10 +1276,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1149,10 +1291,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
@@ -1164,15 +1306,15 @@
         <v>2</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="23"/>
       <c r="D15" s="26"/>
     </row>
-    <row r="16" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
@@ -1196,7 +1338,7 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="323.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="355.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -1208,18 +1350,18 @@
         <v>8</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
@@ -1231,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>27</v>
@@ -1239,12 +1381,12 @@
       <c r="G18" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="34" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
@@ -1256,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>28</v>
@@ -1264,12 +1406,12 @@
       <c r="G19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="34" t="s">
         <v>28</v>
       </c>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -1281,20 +1423,20 @@
         <v>4</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>29</v>
+        <v>63</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
@@ -1306,20 +1448,20 @@
         <v>8</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>30</v>
+        <v>65</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -1331,20 +1473,20 @@
         <v>8</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>31</v>
+        <v>64</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
@@ -1356,20 +1498,20 @@
         <v>8</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>58</v>
       </c>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
@@ -1381,20 +1523,20 @@
         <v>8</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>29</v>
       </c>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
@@ -1406,20 +1548,20 @@
         <v>8</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>21</v>
       </c>
@@ -1431,27 +1573,27 @@
         <v>8</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C27" s="23"/>
       <c r="D27" s="26"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" s="27">
         <f>SUM(C9:C26)</f>
@@ -1463,10 +1605,10 @@
       <c r="E28" s="14"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I29" s="29"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E31" s="2">
         <f ca="1">+E30:L31</f>
         <v>0</v>
@@ -1478,8 +1620,8 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{519E374F-3251-1B43-903E-C51296BBEC24}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{8A53CC01-053C-8044-A53A-5A6A075C3E14}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{8A53CC01-053C-8044-A53A-5A6A075C3E14}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{519E374F-3251-1B43-903E-C51296BBEC24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1495,26 +1637,26 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="2"/>
-    <col min="5" max="5" width="69.28515625" style="2" customWidth="1"/>
-    <col min="6" max="9" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="2"/>
+    <col min="5" max="5" width="69.33203125" style="2" customWidth="1"/>
+    <col min="6" max="9" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -1524,12 +1666,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7">
@@ -1537,12 +1679,12 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="7">
@@ -1550,22 +1692,22 @@
       </c>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="7">
         <v>0.2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -1578,12 +1720,12 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7">
@@ -1591,7 +1733,7 @@
       </c>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
@@ -1609,28 +1751,28 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>

</xml_diff>